<commit_message>
Reviewed index.js, App.js, Login.js, Dashboard.js, Header.js, Sidebar.js
</commit_message>
<xml_diff>
--- a/docs/04_data_design/io_summary.xlsx
+++ b/docs/04_data_design/io_summary.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Farheen\OBE-TRACKING-SYSTEM\docs\04_data_design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00663F81-BAB9-4E55-AF0C-ED8EC561A206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,239 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
+  <si>
+    <t>Module / Feature</t>
+  </si>
+  <si>
+    <t>Input Description</t>
+  </si>
+  <si>
+    <t>Input Source / Role</t>
+  </si>
+  <si>
+    <t>Output Description</t>
+  </si>
+  <si>
+    <t>Output Destination / Role</t>
+  </si>
+  <si>
+    <t>Notes / Reference</t>
+  </si>
+  <si>
+    <t>User Management &amp; Access Control</t>
+  </si>
+  <si>
+    <t>User details (name, email, role, password)</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Success/failure message, audit log</t>
+  </si>
+  <si>
+    <t>Admin, Audit logs</t>
+  </si>
+  <si>
+    <t>FR1–FR5</t>
+  </si>
+  <si>
+    <t>Academic &amp; OBE Master Data</t>
+  </si>
+  <si>
+    <t>Program, Course, Semester, CO/PO/PSO definitions</t>
+  </si>
+  <si>
+    <t>Admin, HOD, Coordinator</t>
+  </si>
+  <si>
+    <t>Confirmation, updated database records</t>
+  </si>
+  <si>
+    <t>FR6–FR10</t>
+  </si>
+  <si>
+    <t>Target Setting &amp; Approval</t>
+  </si>
+  <si>
+    <t>CO/PO/PSO target values</t>
+  </si>
+  <si>
+    <t>HOD, Coordinator</t>
+  </si>
+  <si>
+    <t>Confirmation, updated target records</t>
+  </si>
+  <si>
+    <t>FR11–FR13</t>
+  </si>
+  <si>
+    <t>Assessment Data Entry</t>
+  </si>
+  <si>
+    <t>Marks, assessment type, evidence documents</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Confirmation, updated attainment calculation</t>
+  </si>
+  <si>
+    <t>Faculty, Dashboard</t>
+  </si>
+  <si>
+    <t>FR14–FR18</t>
+  </si>
+  <si>
+    <t>Direct Attainment Calculation</t>
+  </si>
+  <si>
+    <t>Assessment data, configured formulas, weightages</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>CO attainment, attainment gaps</t>
+  </si>
+  <si>
+    <t>Dashboard, Reports</t>
+  </si>
+  <si>
+    <t>FR19–FR22</t>
+  </si>
+  <si>
+    <t>Indirect Attainment Management</t>
+  </si>
+  <si>
+    <t>Survey responses, enrollment number</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>CO/PO/PSO scores</t>
+  </si>
+  <si>
+    <t>FR23–FR29</t>
+  </si>
+  <si>
+    <t>Survey Management</t>
+  </si>
+  <si>
+    <t>Survey questions, responses, anonymous flags</t>
+  </si>
+  <si>
+    <t>HOD, Coordinator, Faculty, Students</t>
+  </si>
+  <si>
+    <t>Survey score, audit log</t>
+  </si>
+  <si>
+    <t>FR30–FR36</t>
+  </si>
+  <si>
+    <t>Stress Analysis &amp; Correlation</t>
+  </si>
+  <si>
+    <t>Stress survey responses, academic data</t>
+  </si>
+  <si>
+    <t>Students, System</t>
+  </si>
+  <si>
+    <t>Stress trends, academic vs non-academic scores</t>
+  </si>
+  <si>
+    <t>FR37–FR41</t>
+  </si>
+  <si>
+    <t>Backtracking &amp; Root Cause Analysis</t>
+  </si>
+  <si>
+    <t>Low attainment data, CO/Assessment mapping</t>
+  </si>
+  <si>
+    <t>Tracing report, contribution percentages</t>
+  </si>
+  <si>
+    <t>FR42–FR45</t>
+  </si>
+  <si>
+    <t>Monthly Attainment Tracking</t>
+  </si>
+  <si>
+    <t>Assessment &amp; survey data</t>
+  </si>
+  <si>
+    <t>Month-wise attainment snapshot</t>
+  </si>
+  <si>
+    <t>FR46–FR49</t>
+  </si>
+  <si>
+    <t>Dashboards &amp; Visualization</t>
+  </si>
+  <si>
+    <t>Attainment, survey, stress data</t>
+  </si>
+  <si>
+    <t>Role-based dashboards</t>
+  </si>
+  <si>
+    <t>Users (Faculty, HOD, Coordinator)</t>
+  </si>
+  <si>
+    <t>FR50–FR53</t>
+  </si>
+  <si>
+    <t>Report Generation &amp; Workflow</t>
+  </si>
+  <si>
+    <t>Data from all modules</t>
+  </si>
+  <si>
+    <t>Audit-ready reports</t>
+  </si>
+  <si>
+    <t>Coordinator, Auditor</t>
+  </si>
+  <si>
+    <t>FR54–FR57</t>
+  </si>
+  <si>
+    <t>System Configuration &amp; History</t>
+  </si>
+  <si>
+    <t>Formulas, thresholds, weightages</t>
+  </si>
+  <si>
+    <t>Updated config logs</t>
+  </si>
+  <si>
+    <t>Dashboard, Audit logs</t>
+  </si>
+  <si>
+    <t>FR58–FR60</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +272,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +280,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +586,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>